<commit_message>
Updated Core API Tests
</commit_message>
<xml_diff>
--- a/tests/artifact/data/CloseBook-RollOver.data.xlsx
+++ b/tests/artifact/data/CloseBook-RollOver.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6910" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -124,90 +124,96 @@
     <t>yearstart</t>
   </si>
   <si>
+    <t>2033-04-01</t>
+  </si>
+  <si>
+    <t>yearend</t>
+  </si>
+  <si>
+    <t>2034-03-31</t>
+  </si>
+  <si>
+    <t>orgstate</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>orgcity</t>
+  </si>
+  <si>
+    <t>Mapusa</t>
+  </si>
+  <si>
+    <t>orgaddr</t>
+  </si>
+  <si>
+    <t>orgpincode</t>
+  </si>
+  <si>
+    <t>403519</t>
+  </si>
+  <si>
+    <t>orgcountry</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>orgtelno</t>
+  </si>
+  <si>
+    <t>1551515525</t>
+  </si>
+  <si>
+    <t>orgfax</t>
+  </si>
+  <si>
+    <t>55545555</t>
+  </si>
+  <si>
+    <t>orgwebsite</t>
+  </si>
+  <si>
+    <t>www.mapusa.com</t>
+  </si>
+  <si>
+    <t>orgemail</t>
+  </si>
+  <si>
+    <t>helpdesk@mapusa.com</t>
+  </si>
+  <si>
+    <t>orgpan</t>
+  </si>
+  <si>
+    <t>APJNS55JKK</t>
+  </si>
+  <si>
+    <t>orgmvat</t>
+  </si>
+  <si>
+    <t>JHJFhhfj838</t>
+  </si>
+  <si>
+    <t>orgstax</t>
+  </si>
+  <si>
+    <t>54565</t>
+  </si>
+  <si>
+    <t>orgregno</t>
+  </si>
+  <si>
+    <t>hfjd849</t>
+  </si>
+  <si>
+    <t>orgregdate</t>
+  </si>
+  <si>
     <t>2023-01-03</t>
   </si>
   <si>
-    <t>yearend</t>
-  </si>
-  <si>
-    <t>orgstate</t>
-  </si>
-  <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>orgcity</t>
-  </si>
-  <si>
-    <t>Mapusa</t>
-  </si>
-  <si>
-    <t>orgaddr</t>
-  </si>
-  <si>
-    <t>orgpincode</t>
-  </si>
-  <si>
-    <t>403519</t>
-  </si>
-  <si>
-    <t>orgcountry</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>orgtelno</t>
-  </si>
-  <si>
-    <t>1551515525</t>
-  </si>
-  <si>
-    <t>orgfax</t>
-  </si>
-  <si>
-    <t>55545555</t>
-  </si>
-  <si>
-    <t>orgwebsite</t>
-  </si>
-  <si>
-    <t>www.mapusa.com</t>
-  </si>
-  <si>
-    <t>orgemail</t>
-  </si>
-  <si>
-    <t>helpdesk@mapusa.com</t>
-  </si>
-  <si>
-    <t>orgpan</t>
-  </si>
-  <si>
-    <t>APJNS55JKK</t>
-  </si>
-  <si>
-    <t>orgmvat</t>
-  </si>
-  <si>
-    <t>JHJFhhfj838</t>
-  </si>
-  <si>
-    <t>orgstax</t>
-  </si>
-  <si>
-    <t>54565</t>
-  </si>
-  <si>
-    <t>orgregno</t>
-  </si>
-  <si>
-    <t>hfjd849</t>
-  </si>
-  <si>
-    <t>orgregdate</t>
-  </si>
-  <si>
     <t>orgfcrano</t>
   </si>
   <si>
@@ -257,6 +263,30 @@
   </si>
   <si>
     <t>logo</t>
+  </si>
+  <si>
+    <t>Startyear</t>
+  </si>
+  <si>
+    <t>2023-04-01</t>
+  </si>
+  <si>
+    <t>Endyear</t>
+  </si>
+  <si>
+    <t>2024-03-31</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>newpassword</t>
+  </si>
+  <si>
+    <t>testclosebook</t>
   </si>
 </sst>
 </file>
@@ -264,10 +294,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -308,6 +338,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -316,17 +384,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -338,38 +400,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,53 +431,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,13 +446,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -460,37 +490,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,145 +670,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,6 +699,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -687,11 +732,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -711,47 +777,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -771,148 +801,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -939,59 +969,59 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1356,8 +1386,8 @@
   <sheetPr/>
   <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -1509,140 +1539,140 @@
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" ht="23.1" customHeight="1" spans="1:2">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" ht="23.1" customHeight="1" spans="1:2">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" ht="23.1" customHeight="1" spans="1:2">
       <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" ht="23.1" customHeight="1" spans="1:2">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" ht="23.1" customHeight="1" spans="1:2">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" ht="23.1" customHeight="1" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" ht="23.1" customHeight="1" spans="1:2">
       <c r="A25" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" ht="23.1" customHeight="1" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" ht="23.1" customHeight="1" spans="1:2">
       <c r="A27" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" ht="23.1" customHeight="1" spans="1:2">
       <c r="A28" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" ht="23.1" customHeight="1" spans="1:2">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" ht="23.1" customHeight="1" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" ht="23.1" customHeight="1" spans="1:2">
       <c r="A31" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" ht="23.1" customHeight="1" spans="1:2">
       <c r="A32" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" ht="23.1" customHeight="1" spans="1:2">
       <c r="A33" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" ht="23.1" customHeight="1" spans="1:2">
       <c r="A34" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" ht="23.1" customHeight="1" spans="1:2">
       <c r="A35" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>3</v>
@@ -1650,7 +1680,7 @@
     </row>
     <row r="36" ht="23.1" customHeight="1" spans="1:2">
       <c r="A36" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>3</v>
@@ -1658,7 +1688,7 @@
     </row>
     <row r="37" ht="23.1" customHeight="1" spans="1:2">
       <c r="A37" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>3</v>
@@ -1666,7 +1696,7 @@
     </row>
     <row r="38" ht="23.1" customHeight="1" spans="1:2">
       <c r="A38" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -1674,15 +1704,15 @@
     </row>
     <row r="39" ht="23.1" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" ht="23.1" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>3</v>
@@ -1690,7 +1720,7 @@
     </row>
     <row r="41" ht="23.1" customHeight="1" spans="1:2">
       <c r="A41" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>3</v>
@@ -1698,55 +1728,75 @@
     </row>
     <row r="42" ht="23.1" customHeight="1" spans="1:2">
       <c r="A42" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" ht="23.1" customHeight="1" spans="1:2">
       <c r="A43" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" ht="23.1" customHeight="1" spans="1:2">
       <c r="A44" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" ht="23.1" customHeight="1" spans="1:2">
       <c r="A45" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" ht="23.1" customHeight="1" spans="1:2">
       <c r="A46" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A48" s="4"/>
-    </row>
-    <row r="49" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A50" s="4"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="51" ht="23.1" customHeight="1" spans="1:1">
       <c r="A51" s="4"/>

</xml_diff>

<commit_message>
tests: Updated Core API Tests
</commit_message>
<xml_diff>
--- a/tests/artifact/data/CloseBook-RollOver.data.xlsx
+++ b/tests/artifact/data/CloseBook-RollOver.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6910" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -124,90 +124,96 @@
     <t>yearstart</t>
   </si>
   <si>
+    <t>2033-04-01</t>
+  </si>
+  <si>
+    <t>yearend</t>
+  </si>
+  <si>
+    <t>2034-03-31</t>
+  </si>
+  <si>
+    <t>orgstate</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>orgcity</t>
+  </si>
+  <si>
+    <t>Mapusa</t>
+  </si>
+  <si>
+    <t>orgaddr</t>
+  </si>
+  <si>
+    <t>orgpincode</t>
+  </si>
+  <si>
+    <t>403519</t>
+  </si>
+  <si>
+    <t>orgcountry</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>orgtelno</t>
+  </si>
+  <si>
+    <t>1551515525</t>
+  </si>
+  <si>
+    <t>orgfax</t>
+  </si>
+  <si>
+    <t>55545555</t>
+  </si>
+  <si>
+    <t>orgwebsite</t>
+  </si>
+  <si>
+    <t>www.mapusa.com</t>
+  </si>
+  <si>
+    <t>orgemail</t>
+  </si>
+  <si>
+    <t>helpdesk@mapusa.com</t>
+  </si>
+  <si>
+    <t>orgpan</t>
+  </si>
+  <si>
+    <t>APJNS55JKK</t>
+  </si>
+  <si>
+    <t>orgmvat</t>
+  </si>
+  <si>
+    <t>JHJFhhfj838</t>
+  </si>
+  <si>
+    <t>orgstax</t>
+  </si>
+  <si>
+    <t>54565</t>
+  </si>
+  <si>
+    <t>orgregno</t>
+  </si>
+  <si>
+    <t>hfjd849</t>
+  </si>
+  <si>
+    <t>orgregdate</t>
+  </si>
+  <si>
     <t>2023-01-03</t>
   </si>
   <si>
-    <t>yearend</t>
-  </si>
-  <si>
-    <t>orgstate</t>
-  </si>
-  <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>orgcity</t>
-  </si>
-  <si>
-    <t>Mapusa</t>
-  </si>
-  <si>
-    <t>orgaddr</t>
-  </si>
-  <si>
-    <t>orgpincode</t>
-  </si>
-  <si>
-    <t>403519</t>
-  </si>
-  <si>
-    <t>orgcountry</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>orgtelno</t>
-  </si>
-  <si>
-    <t>1551515525</t>
-  </si>
-  <si>
-    <t>orgfax</t>
-  </si>
-  <si>
-    <t>55545555</t>
-  </si>
-  <si>
-    <t>orgwebsite</t>
-  </si>
-  <si>
-    <t>www.mapusa.com</t>
-  </si>
-  <si>
-    <t>orgemail</t>
-  </si>
-  <si>
-    <t>helpdesk@mapusa.com</t>
-  </si>
-  <si>
-    <t>orgpan</t>
-  </si>
-  <si>
-    <t>APJNS55JKK</t>
-  </si>
-  <si>
-    <t>orgmvat</t>
-  </si>
-  <si>
-    <t>JHJFhhfj838</t>
-  </si>
-  <si>
-    <t>orgstax</t>
-  </si>
-  <si>
-    <t>54565</t>
-  </si>
-  <si>
-    <t>orgregno</t>
-  </si>
-  <si>
-    <t>hfjd849</t>
-  </si>
-  <si>
-    <t>orgregdate</t>
-  </si>
-  <si>
     <t>orgfcrano</t>
   </si>
   <si>
@@ -257,6 +263,30 @@
   </si>
   <si>
     <t>logo</t>
+  </si>
+  <si>
+    <t>Startyear</t>
+  </si>
+  <si>
+    <t>2023-04-01</t>
+  </si>
+  <si>
+    <t>Endyear</t>
+  </si>
+  <si>
+    <t>2024-03-31</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>newpassword</t>
+  </si>
+  <si>
+    <t>testclosebook</t>
   </si>
 </sst>
 </file>
@@ -264,10 +294,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -308,6 +338,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -316,17 +384,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -338,38 +400,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,53 +431,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,13 +446,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -460,37 +490,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,145 +670,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,6 +699,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -687,11 +732,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -711,47 +777,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -771,148 +801,148 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -939,59 +969,59 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1356,8 +1386,8 @@
   <sheetPr/>
   <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -1509,140 +1539,140 @@
         <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" ht="23.1" customHeight="1" spans="1:2">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" ht="23.1" customHeight="1" spans="1:2">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" ht="23.1" customHeight="1" spans="1:2">
       <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" ht="23.1" customHeight="1" spans="1:2">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" ht="23.1" customHeight="1" spans="1:2">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" ht="23.1" customHeight="1" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" ht="23.1" customHeight="1" spans="1:2">
       <c r="A25" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" ht="23.1" customHeight="1" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" ht="23.1" customHeight="1" spans="1:2">
       <c r="A27" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" ht="23.1" customHeight="1" spans="1:2">
       <c r="A28" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" ht="23.1" customHeight="1" spans="1:2">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" ht="23.1" customHeight="1" spans="1:2">
       <c r="A30" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" ht="23.1" customHeight="1" spans="1:2">
       <c r="A31" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" ht="23.1" customHeight="1" spans="1:2">
       <c r="A32" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" ht="23.1" customHeight="1" spans="1:2">
       <c r="A33" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" ht="23.1" customHeight="1" spans="1:2">
       <c r="A34" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" ht="23.1" customHeight="1" spans="1:2">
       <c r="A35" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>3</v>
@@ -1650,7 +1680,7 @@
     </row>
     <row r="36" ht="23.1" customHeight="1" spans="1:2">
       <c r="A36" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>3</v>
@@ -1658,7 +1688,7 @@
     </row>
     <row r="37" ht="23.1" customHeight="1" spans="1:2">
       <c r="A37" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>3</v>
@@ -1666,7 +1696,7 @@
     </row>
     <row r="38" ht="23.1" customHeight="1" spans="1:2">
       <c r="A38" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -1674,15 +1704,15 @@
     </row>
     <row r="39" ht="23.1" customHeight="1" spans="1:2">
       <c r="A39" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" ht="23.1" customHeight="1" spans="1:2">
       <c r="A40" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>3</v>
@@ -1690,7 +1720,7 @@
     </row>
     <row r="41" ht="23.1" customHeight="1" spans="1:2">
       <c r="A41" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>3</v>
@@ -1698,55 +1728,75 @@
     </row>
     <row r="42" ht="23.1" customHeight="1" spans="1:2">
       <c r="A42" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" ht="23.1" customHeight="1" spans="1:2">
       <c r="A43" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" ht="23.1" customHeight="1" spans="1:2">
       <c r="A44" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" ht="23.1" customHeight="1" spans="1:2">
       <c r="A45" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" ht="23.1" customHeight="1" spans="1:2">
       <c r="A46" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A47" s="4"/>
-    </row>
-    <row r="48" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A48" s="4"/>
-    </row>
-    <row r="49" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A50" s="4"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A50" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="51" ht="23.1" customHeight="1" spans="1:1">
       <c r="A51" s="4"/>

</xml_diff>

<commit_message>
add script for Accounts and Closebook-Rollover Modules
</commit_message>
<xml_diff>
--- a/tests/artifact/data/CloseBook-RollOver.data.xlsx
+++ b/tests/artifact/data/CloseBook-RollOver.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -136,7 +136,7 @@
     <t>orgstate</t>
   </si>
   <si>
-    <t>Goa</t>
+    <t>Bangalore</t>
   </si>
   <si>
     <t>orgcity</t>
@@ -280,13 +280,16 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
     <t>newpassword</t>
   </si>
   <si>
     <t>testclosebook@123</t>
+  </si>
+  <si>
+    <t>Negative.closebook</t>
+  </si>
+  <si>
+    <t>31-02-2024,02-31-2024,123, ,,string123,@,etc</t>
   </si>
 </sst>
 </file>
@@ -1386,14 +1389,14 @@
   <sheetPr/>
   <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="34.9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.2857142857143" style="2" customWidth="1"/>
     <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
     <col min="6" max="16384" width="10.7" style="3"/>
   </cols>
@@ -1787,19 +1790,24 @@
         <v>80</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" ht="23.1" customHeight="1" spans="1:2">
       <c r="A50" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B50" s="6" t="s">
+    </row>
+    <row r="51" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A51" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="51" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A51" s="4"/>
+      <c r="B51" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="52" ht="23.1" customHeight="1" spans="1:1">
       <c r="A52" s="4"/>

</xml_diff>

<commit_message>
Updated the Close books roll over script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/CloseBook-RollOver.data.xlsx
+++ b/tests/artifact/data/CloseBook-RollOver.data.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>testclosebook</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1412,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -1825,8 +1831,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A52" s="4"/>
+    <row r="52" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A52" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="53" ht="23.1" customHeight="1" spans="1:1">
       <c r="A53" s="4"/>

</xml_diff>